<commit_message>
Realization of the MD
</commit_message>
<xml_diff>
--- a/doc/Sprint1/1201371/MeasuresTable.xlsx
+++ b/doc/Sprint1/1201371/MeasuresTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\transferencias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rcomp\doc\Sprint1\1201371\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C460D7-BBBE-4193-97EA-7A6B4CD89454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF620769-B286-4443-9104-C87AF42E3799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EEC54CBA-3F04-432E-8C8C-49267990381D}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{EEC54CBA-3F04-432E-8C8C-49267990381D}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -666,7 +666,7 @@
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,8 +820,8 @@
         <v>168.02709999999996</v>
       </c>
       <c r="F8" s="28">
-        <f ca="1">SUM(F3:F8)</f>
-        <v>38</v>
+        <f>SUM(F3:F7)</f>
+        <v>44</v>
       </c>
       <c r="N8" s="12"/>
       <c r="O8" s="14"/>

</xml_diff>